<commit_message>
Refinements for LOBDBase Expansion
CholestorolActetate entries corrected to CholesterolAcetate.

Updated default database, componentcomptable and adduct hierarchies objects in line with the above.

generateLOBdbase.R - corrected comments reference Si instead of D or C_thirteen. Added line breaks to comply with bioc style guide.
</commit_message>
<xml_diff>
--- a/inst/doc/xlsx/LOBSTAHS_adductHierarchies.xlsx
+++ b/inst/doc/xlsx/LOBSTAHS_adductHierarchies.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\R\LOBDBase Update, MAG, DAG, Lyso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox\R\LOBDBase Update, MAG, DAG, Lyso\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LOBSTAHS_adductHierarchies" sheetId="5" r:id="rId1"/>
@@ -279,9 +279,6 @@
     <t>WaxEster</t>
   </si>
   <si>
-    <t>ChlorestorolAcetate</t>
-  </si>
-  <si>
     <t>diglycerides</t>
   </si>
   <si>
@@ -301,6 +298,9 @@
   </si>
   <si>
     <t>Added MAG, DAG, LysoIP_DAGs, Cholesterol/Coprostanols and esters, Astaxanthin, Bile Salts, Support for 2H and 13C Isotopes.</t>
+  </si>
+  <si>
+    <t>ChloresterolAcetate</t>
   </si>
 </sst>
 </file>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AS5" sqref="AS5"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -940,25 +940,25 @@
         <v>82</v>
       </c>
       <c r="AJ2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK2" t="s">
         <v>83</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM2" t="s">
         <v>84</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AN2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AP2" t="s">
         <v>88</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.25">
@@ -2064,8 +2064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2245,10 +2245,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>42925</v>
+        <v>42964</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Fixing spelling errors on input tables
</commit_message>
<xml_diff>
--- a/inst/doc/xlsx/LOBSTAHS_adductHierarchies.xlsx
+++ b/inst/doc/xlsx/LOBSTAHS_adductHierarchies.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox\R\LOBDBase Update, MAG, DAG, Lyso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesrco/Code/LOBSTAHS/inst/doc/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="39020" yWindow="-1580" windowWidth="32940" windowHeight="18440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LOBSTAHS_adductHierarchies" sheetId="5" r:id="rId1"/>
@@ -300,13 +300,13 @@
     <t>Added MAG, DAG, LysoIP_DAGs, Cholesterol/Coprostanols and esters, Astaxanthin, Bile Salts, Support for 2H and 13C Isotopes.</t>
   </si>
   <si>
-    <t>ChloresterolAcetate</t>
+    <t>CholesterolAcetate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -788,17 +788,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP22"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V24" sqref="V24"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AP3" sqref="AP3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.875" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
       <c r="C1" s="4" t="s">
         <v>47</v>
       </c>
@@ -832,8 +832,17 @@
       <c r="AE1" s="4"/>
       <c r="AF1" s="4"/>
       <c r="AG1" s="4"/>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="4"/>
+      <c r="AJ1" s="4"/>
+      <c r="AK1" s="4"/>
+      <c r="AL1" s="4"/>
+      <c r="AM1" s="4"/>
+      <c r="AN1" s="4"/>
+      <c r="AO1" s="4"/>
+      <c r="AP1" s="4"/>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2053,7 +2062,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:AG1"/>
+    <mergeCell ref="C1:AP1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -2064,11 +2073,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="74.5" customWidth="1"/>
@@ -2087,7 +2096,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
Revert "Fixing spelling errors on input tables"
This reverts commit f4ce77735c8e33886c7cde4a06dbbdee4eaf6e90.
</commit_message>
<xml_diff>
--- a/inst/doc/xlsx/LOBSTAHS_adductHierarchies.xlsx
+++ b/inst/doc/xlsx/LOBSTAHS_adductHierarchies.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesrco/Code/LOBSTAHS/inst/doc/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox\R\LOBDBase Update, MAG, DAG, Lyso\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="39020" yWindow="-1580" windowWidth="32940" windowHeight="18440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LOBSTAHS_adductHierarchies" sheetId="5" r:id="rId1"/>
@@ -300,13 +300,13 @@
     <t>Added MAG, DAG, LysoIP_DAGs, Cholesterol/Coprostanols and esters, Astaxanthin, Bile Salts, Support for 2H and 13C Isotopes.</t>
   </si>
   <si>
-    <t>CholesterolAcetate</t>
+    <t>ChloresterolAcetate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -788,17 +788,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AP3" sqref="AP3"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="C1" s="4" t="s">
         <v>47</v>
       </c>
@@ -832,17 +832,8 @@
       <c r="AE1" s="4"/>
       <c r="AF1" s="4"/>
       <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
-      <c r="AK1" s="4"/>
-      <c r="AL1" s="4"/>
-      <c r="AM1" s="4"/>
-      <c r="AN1" s="4"/>
-      <c r="AO1" s="4"/>
-      <c r="AP1" s="4"/>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2062,7 +2053,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:AP1"/>
+    <mergeCell ref="C1:AG1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -2073,11 +2064,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="74.5" customWidth="1"/>
@@ -2096,7 +2087,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
Fixing spelling error in new compTable and adductHierarchies
</commit_message>
<xml_diff>
--- a/inst/doc/xlsx/LOBSTAHS_adductHierarchies.xlsx
+++ b/inst/doc/xlsx/LOBSTAHS_adductHierarchies.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox\R\LOBDBase Update, MAG, DAG, Lyso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesrco/Code/LOBSTAHS/inst/doc/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="40360" yWindow="-460" windowWidth="28800" windowHeight="12480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LOBSTAHS_adductHierarchies" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="92">
   <si>
     <t>DGCC</t>
   </si>
@@ -300,13 +300,16 @@
     <t>Added MAG, DAG, LysoIP_DAGs, Cholesterol/Coprostanols and esters, Astaxanthin, Bile Salts, Support for 2H and 13C Isotopes.</t>
   </si>
   <si>
-    <t>ChloresterolAcetate</t>
+    <t>CholesterolAcetate</t>
+  </si>
+  <si>
+    <t>Fixed spelling error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -789,13 +792,13 @@
   <dimension ref="A1:AP22"/>
   <sheetViews>
     <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V24" sqref="V24"/>
+      <selection activeCell="AJ3" sqref="AJ3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.875" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.25">
@@ -2062,13 +2065,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="74.5" customWidth="1"/>
@@ -2087,7 +2090,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>68</v>
       </c>
@@ -2252,6 +2255,17 @@
       </c>
       <c r="C24" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>42965</v>
+      </c>
+      <c r="B25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
xlsx file update to include PA and LPA
</commit_message>
<xml_diff>
--- a/inst/doc/xlsx/LOBSTAHS_adductHierarchies.xlsx
+++ b/inst/doc/xlsx/LOBSTAHS_adductHierarchies.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesrco/Code/LOBSTAHS/inst/doc/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox\R\LOBSTAHS-JEH\inst\doc\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40360" yWindow="-460" windowWidth="28800" windowHeight="12480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12030" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LOBSTAHS_adductHierarchies" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="94">
   <si>
     <t>DGCC</t>
   </si>
@@ -304,12 +304,18 @@
   </si>
   <si>
     <t>Fixed spelling error</t>
+  </si>
+  <si>
+    <t>Added PA and LPA, estimated hierarchies.</t>
+  </si>
+  <si>
+    <t>PA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -789,19 +795,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP22"/>
+  <dimension ref="A1:AQ22"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AJ3" sqref="AJ3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="C1" s="4" t="s">
         <v>47</v>
       </c>
@@ -835,8 +841,9 @@
       <c r="AE1" s="4"/>
       <c r="AF1" s="4"/>
       <c r="AG1" s="4"/>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AH1" s="4"/>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -871,100 +878,103 @@
         <v>49</v>
       </c>
       <c r="L2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M2" t="s">
         <v>14</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>20</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>15</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>16</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>80</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>81</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>51</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>52</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>53</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>54</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>55</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>56</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>57</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>59</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>58</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>60</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>61</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>62</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>63</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>64</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>65</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>79</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>82</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>90</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>83</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>87</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>84</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>85</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>86</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1007,47 +1017,50 @@
       <c r="O3">
         <v>1</v>
       </c>
-      <c r="Q3">
+      <c r="P3">
         <v>1</v>
       </c>
       <c r="R3">
         <v>1</v>
       </c>
       <c r="S3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="T3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U3">
-        <v>2</v>
-      </c>
-      <c r="W3">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>2</v>
       </c>
       <c r="X3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Y3">
-        <v>3</v>
-      </c>
-      <c r="AA3">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>3</v>
       </c>
       <c r="AB3">
-        <v>1</v>
-      </c>
-      <c r="AE3">
+        <v>2</v>
+      </c>
+      <c r="AC3">
         <v>1</v>
       </c>
       <c r="AF3">
         <v>1</v>
       </c>
-      <c r="AP3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AQ3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1057,11 +1070,11 @@
       <c r="G4">
         <v>3</v>
       </c>
-      <c r="X4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="Y4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1089,23 +1102,23 @@
       <c r="K5">
         <v>3</v>
       </c>
-      <c r="S5">
-        <v>3</v>
-      </c>
-      <c r="U5">
+      <c r="T5">
         <v>3</v>
       </c>
       <c r="V5">
         <v>3</v>
       </c>
-      <c r="Y5">
-        <v>2</v>
+      <c r="W5">
+        <v>3</v>
       </c>
       <c r="Z5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="AA5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1115,11 +1128,11 @@
       <c r="G6">
         <v>5</v>
       </c>
-      <c r="M6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1147,10 +1160,7 @@
       <c r="K7">
         <v>1</v>
       </c>
-      <c r="S7">
-        <v>1</v>
-      </c>
-      <c r="U7">
+      <c r="T7">
         <v>1</v>
       </c>
       <c r="V7">
@@ -1159,7 +1169,7 @@
       <c r="W7">
         <v>1</v>
       </c>
-      <c r="Y7">
+      <c r="X7">
         <v>1</v>
       </c>
       <c r="Z7">
@@ -1168,8 +1178,11 @@
       <c r="AA7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AB7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1179,26 +1192,26 @@
       <c r="G8">
         <v>2</v>
       </c>
-      <c r="L8">
-        <v>2</v>
-      </c>
       <c r="M8">
         <v>2</v>
       </c>
-      <c r="O8">
-        <v>2</v>
-      </c>
-      <c r="S8">
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="P8">
+        <v>2</v>
+      </c>
+      <c r="T8">
         <v>8</v>
       </c>
-      <c r="T8">
-        <v>2</v>
-      </c>
       <c r="U8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="V8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1208,23 +1221,23 @@
       <c r="G9">
         <v>4</v>
       </c>
-      <c r="L9">
-        <v>3</v>
-      </c>
       <c r="M9">
         <v>3</v>
       </c>
-      <c r="O9">
-        <v>3</v>
-      </c>
-      <c r="S9">
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="P9">
+        <v>3</v>
+      </c>
+      <c r="T9">
         <v>9</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1252,20 +1265,20 @@
       <c r="K10">
         <v>5</v>
       </c>
-      <c r="S10">
-        <v>6</v>
-      </c>
-      <c r="V10">
-        <v>5</v>
+      <c r="T10">
+        <v>6</v>
       </c>
       <c r="W10">
         <v>5</v>
       </c>
-      <c r="Z10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="X10">
+        <v>5</v>
+      </c>
+      <c r="AA10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1293,26 +1306,26 @@
       <c r="K11">
         <v>2</v>
       </c>
-      <c r="S11">
-        <v>2</v>
-      </c>
-      <c r="V11">
+      <c r="T11">
         <v>2</v>
       </c>
       <c r="W11">
         <v>2</v>
       </c>
-      <c r="Y11">
-        <v>4</v>
+      <c r="X11">
+        <v>2</v>
       </c>
       <c r="Z11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AA11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="AB11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1340,23 +1353,23 @@
       <c r="K12">
         <v>6</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>7</v>
       </c>
-      <c r="U12">
-        <v>6</v>
-      </c>
       <c r="V12">
         <v>6</v>
       </c>
       <c r="W12">
         <v>6</v>
       </c>
-      <c r="Z12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="X12">
+        <v>6</v>
+      </c>
+      <c r="AA12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1384,29 +1397,29 @@
       <c r="K13">
         <v>4</v>
       </c>
-      <c r="S13">
-        <v>4</v>
-      </c>
-      <c r="U13">
+      <c r="T13">
         <v>4</v>
       </c>
       <c r="V13">
         <v>4</v>
       </c>
       <c r="W13">
-        <v>3</v>
-      </c>
-      <c r="Y13">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="X13">
+        <v>3</v>
       </c>
       <c r="Z13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AA13">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AB13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1431,20 +1444,17 @@
       <c r="K14">
         <v>1</v>
       </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
       <c r="M14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O14">
-        <v>4</v>
-      </c>
-      <c r="S14">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>4</v>
       </c>
       <c r="T14">
         <v>1</v>
@@ -1453,10 +1463,10 @@
         <v>1</v>
       </c>
       <c r="V14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X14">
         <v>1</v>
@@ -1474,43 +1484,46 @@
         <v>1</v>
       </c>
       <c r="AC14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AD14">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AE14">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AF14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AG14">
         <v>1</v>
       </c>
-      <c r="AI14">
-        <v>2</v>
+      <c r="AH14">
+        <v>1</v>
       </c>
       <c r="AJ14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AL14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AM14">
         <v>1</v>
       </c>
       <c r="AN14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AO14">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AP14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1538,13 +1551,10 @@
       <c r="K15">
         <v>5</v>
       </c>
-      <c r="L15">
-        <v>5</v>
-      </c>
       <c r="M15">
-        <v>6</v>
-      </c>
-      <c r="O15">
+        <v>5</v>
+      </c>
+      <c r="N15">
         <v>6</v>
       </c>
       <c r="P15">
@@ -1557,43 +1567,43 @@
         <v>6</v>
       </c>
       <c r="S15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="T15">
         <v>7</v>
       </c>
       <c r="U15">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="V15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W15">
-        <v>5</v>
-      </c>
-      <c r="Z15">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="X15">
+        <v>5</v>
       </c>
       <c r="AA15">
         <v>4</v>
       </c>
       <c r="AB15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AC15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AD15">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AE15">
-        <v>6</v>
-      </c>
-      <c r="AI15">
-        <v>4</v>
-      </c>
-      <c r="AK15">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="AF15">
+        <v>6</v>
+      </c>
+      <c r="AJ15">
+        <v>4</v>
       </c>
       <c r="AL15">
         <v>3</v>
@@ -1607,8 +1617,11 @@
       <c r="AO15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AP15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1624,10 +1637,10 @@
       <c r="I16">
         <v>1</v>
       </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
-      <c r="O16">
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="N16">
         <v>1</v>
       </c>
       <c r="P16">
@@ -1640,22 +1653,22 @@
         <v>1</v>
       </c>
       <c r="S16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V16">
-        <v>4</v>
-      </c>
-      <c r="AB16">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="W16">
+        <v>4</v>
       </c>
       <c r="AC16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD16">
         <v>1</v>
@@ -1663,26 +1676,29 @@
       <c r="AE16">
         <v>1</v>
       </c>
-      <c r="AH16">
+      <c r="AF16">
         <v>1</v>
       </c>
       <c r="AI16">
         <v>1</v>
       </c>
-      <c r="AK16">
-        <v>1</v>
-      </c>
-      <c r="AN16">
-        <v>2</v>
+      <c r="AJ16">
+        <v>1</v>
+      </c>
+      <c r="AL16">
+        <v>1</v>
       </c>
       <c r="AO16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AP16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1713,13 +1729,10 @@
       <c r="K17">
         <v>2</v>
       </c>
-      <c r="L17">
-        <v>2</v>
-      </c>
       <c r="M17">
         <v>2</v>
       </c>
-      <c r="O17">
+      <c r="N17">
         <v>2</v>
       </c>
       <c r="P17">
@@ -1741,13 +1754,13 @@
         <v>2</v>
       </c>
       <c r="V17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W17">
-        <v>3</v>
-      </c>
-      <c r="Y17">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="X17">
+        <v>3</v>
       </c>
       <c r="Z17">
         <v>2</v>
@@ -1756,25 +1769,25 @@
         <v>2</v>
       </c>
       <c r="AB17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AC17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD17">
         <v>2</v>
       </c>
       <c r="AE17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AF17">
-        <v>2</v>
-      </c>
-      <c r="AI17">
-        <v>3</v>
-      </c>
-      <c r="AK17">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="AG17">
+        <v>2</v>
+      </c>
+      <c r="AJ17">
+        <v>3</v>
       </c>
       <c r="AL17">
         <v>2</v>
@@ -1783,13 +1796,16 @@
         <v>2</v>
       </c>
       <c r="AN17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AO17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="AP17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1817,38 +1833,38 @@
       <c r="K18">
         <v>4</v>
       </c>
-      <c r="L18">
-        <v>3</v>
-      </c>
       <c r="M18">
-        <v>4</v>
-      </c>
-      <c r="O18">
-        <v>3</v>
-      </c>
-      <c r="S18">
+        <v>3</v>
+      </c>
+      <c r="N18">
+        <v>4</v>
+      </c>
+      <c r="P18">
+        <v>3</v>
+      </c>
+      <c r="T18">
         <v>8</v>
       </c>
-      <c r="T18">
-        <v>3</v>
-      </c>
-      <c r="V18">
+      <c r="U18">
+        <v>3</v>
+      </c>
+      <c r="W18">
         <v>7</v>
       </c>
-      <c r="W18">
-        <v>6</v>
-      </c>
-      <c r="AD18">
+      <c r="X18">
+        <v>6</v>
+      </c>
+      <c r="AE18">
         <v>9</v>
       </c>
-      <c r="AJ18">
-        <v>3</v>
-      </c>
       <c r="AK18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="AL18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1876,17 +1892,14 @@
       <c r="K19">
         <v>3</v>
       </c>
-      <c r="L19">
-        <v>4</v>
-      </c>
       <c r="M19">
-        <v>5</v>
-      </c>
-      <c r="O19">
+        <v>4</v>
+      </c>
+      <c r="N19">
         <v>5</v>
       </c>
       <c r="P19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q19">
         <v>4</v>
@@ -1895,16 +1908,16 @@
         <v>4</v>
       </c>
       <c r="S19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T19">
         <v>5</v>
       </c>
       <c r="U19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="V19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W19">
         <v>2</v>
@@ -1913,40 +1926,40 @@
         <v>2</v>
       </c>
       <c r="Y19">
-        <v>4</v>
-      </c>
-      <c r="AA19">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="Z19">
+        <v>4</v>
       </c>
       <c r="AB19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AC19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE19">
-        <v>2</v>
-      </c>
-      <c r="AI19">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="AF19">
+        <v>2</v>
       </c>
       <c r="AJ19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="AK19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
       <c r="B20" t="s">
         <v>43</v>
       </c>
-      <c r="P20">
-        <v>5</v>
-      </c>
       <c r="Q20">
         <v>5</v>
       </c>
@@ -1954,7 +1967,7 @@
         <v>5</v>
       </c>
       <c r="S20">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T20">
         <v>6</v>
@@ -1963,66 +1976,66 @@
         <v>6</v>
       </c>
       <c r="V20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W20">
+        <v>5</v>
+      </c>
+      <c r="X20">
         <v>7</v>
       </c>
-      <c r="Y20">
-        <v>5</v>
-      </c>
       <c r="Z20">
         <v>5</v>
       </c>
-      <c r="AC20">
+      <c r="AA20">
         <v>5</v>
       </c>
       <c r="AD20">
         <v>5</v>
       </c>
       <c r="AE20">
+        <v>5</v>
+      </c>
+      <c r="AF20">
         <v>7</v>
       </c>
-      <c r="AI20">
-        <v>6</v>
-      </c>
       <c r="AJ20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="AK20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
       <c r="B21" t="s">
         <v>43</v>
       </c>
-      <c r="P21">
-        <v>7</v>
-      </c>
       <c r="Q21">
         <v>7</v>
       </c>
       <c r="R21">
         <v>7</v>
       </c>
-      <c r="AD21">
+      <c r="S21">
+        <v>7</v>
+      </c>
+      <c r="AE21">
         <v>8</v>
       </c>
-      <c r="AJ21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AK21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
       <c r="B22" t="s">
         <v>43</v>
       </c>
-      <c r="P22">
-        <v>3</v>
-      </c>
       <c r="Q22">
         <v>3</v>
       </c>
@@ -2030,16 +2043,16 @@
         <v>3</v>
       </c>
       <c r="S22">
-        <v>4</v>
-      </c>
-      <c r="U22">
+        <v>3</v>
+      </c>
+      <c r="T22">
+        <v>4</v>
+      </c>
+      <c r="V22">
         <v>7</v>
       </c>
-      <c r="W22">
-        <v>4</v>
-      </c>
-      <c r="Y22">
-        <v>3</v>
+      <c r="X22">
+        <v>4</v>
       </c>
       <c r="Z22">
         <v>3</v>
@@ -2047,16 +2060,19 @@
       <c r="AA22">
         <v>3</v>
       </c>
-      <c r="AD22">
+      <c r="AB22">
+        <v>3</v>
+      </c>
+      <c r="AE22">
         <v>7</v>
       </c>
-      <c r="AE22">
+      <c r="AF22">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:AG1"/>
+    <mergeCell ref="C1:AH1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -2065,24 +2081,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="74.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -2090,42 +2106,42 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -2136,7 +2152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>42327</v>
       </c>
@@ -2147,7 +2163,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>42344</v>
       </c>
@@ -2158,7 +2174,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>42403</v>
       </c>
@@ -2169,7 +2185,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>42607</v>
       </c>
@@ -2180,7 +2196,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>42624</v>
       </c>
@@ -2191,7 +2207,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>42709</v>
       </c>
@@ -2202,7 +2218,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>42719</v>
       </c>
@@ -2213,7 +2229,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>42758</v>
       </c>
@@ -2224,7 +2240,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>42769</v>
       </c>
@@ -2235,7 +2251,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>42779</v>
       </c>
@@ -2246,7 +2262,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>42964</v>
       </c>
@@ -2257,7 +2273,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>42965</v>
       </c>
@@ -2266,6 +2282,14 @@
       </c>
       <c r="C25" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>43013</v>
+      </c>
+      <c r="B26" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addition of PA and LPA to LOBdb (#30)
* Update of RData files to include PA and LPA

* CSV file update to include PA and LPA

* xlsx file update to include PA and LPA
</commit_message>
<xml_diff>
--- a/inst/doc/xlsx/LOBSTAHS_adductHierarchies.xlsx
+++ b/inst/doc/xlsx/LOBSTAHS_adductHierarchies.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesrco/Code/LOBSTAHS/inst/doc/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox\R\LOBSTAHS-JEH\inst\doc\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40360" yWindow="-460" windowWidth="28800" windowHeight="12480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12030" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LOBSTAHS_adductHierarchies" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="94">
   <si>
     <t>DGCC</t>
   </si>
@@ -304,12 +304,18 @@
   </si>
   <si>
     <t>Fixed spelling error</t>
+  </si>
+  <si>
+    <t>Added PA and LPA, estimated hierarchies.</t>
+  </si>
+  <si>
+    <t>PA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -789,19 +795,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP22"/>
+  <dimension ref="A1:AQ22"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AJ3" sqref="AJ3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="C1" s="4" t="s">
         <v>47</v>
       </c>
@@ -835,8 +841,9 @@
       <c r="AE1" s="4"/>
       <c r="AF1" s="4"/>
       <c r="AG1" s="4"/>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AH1" s="4"/>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -871,100 +878,103 @@
         <v>49</v>
       </c>
       <c r="L2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M2" t="s">
         <v>14</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>20</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>15</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>16</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>80</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>81</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>51</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>52</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>53</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>54</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>55</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>56</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>57</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>59</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>58</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>60</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>61</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>62</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>63</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>64</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>65</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>79</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>82</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>90</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>83</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>87</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>84</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>85</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>86</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1007,47 +1017,50 @@
       <c r="O3">
         <v>1</v>
       </c>
-      <c r="Q3">
+      <c r="P3">
         <v>1</v>
       </c>
       <c r="R3">
         <v>1</v>
       </c>
       <c r="S3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="T3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U3">
-        <v>2</v>
-      </c>
-      <c r="W3">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>2</v>
       </c>
       <c r="X3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Y3">
-        <v>3</v>
-      </c>
-      <c r="AA3">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>3</v>
       </c>
       <c r="AB3">
-        <v>1</v>
-      </c>
-      <c r="AE3">
+        <v>2</v>
+      </c>
+      <c r="AC3">
         <v>1</v>
       </c>
       <c r="AF3">
         <v>1</v>
       </c>
-      <c r="AP3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AQ3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1057,11 +1070,11 @@
       <c r="G4">
         <v>3</v>
       </c>
-      <c r="X4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="Y4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1089,23 +1102,23 @@
       <c r="K5">
         <v>3</v>
       </c>
-      <c r="S5">
-        <v>3</v>
-      </c>
-      <c r="U5">
+      <c r="T5">
         <v>3</v>
       </c>
       <c r="V5">
         <v>3</v>
       </c>
-      <c r="Y5">
-        <v>2</v>
+      <c r="W5">
+        <v>3</v>
       </c>
       <c r="Z5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="AA5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1115,11 +1128,11 @@
       <c r="G6">
         <v>5</v>
       </c>
-      <c r="M6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1147,10 +1160,7 @@
       <c r="K7">
         <v>1</v>
       </c>
-      <c r="S7">
-        <v>1</v>
-      </c>
-      <c r="U7">
+      <c r="T7">
         <v>1</v>
       </c>
       <c r="V7">
@@ -1159,7 +1169,7 @@
       <c r="W7">
         <v>1</v>
       </c>
-      <c r="Y7">
+      <c r="X7">
         <v>1</v>
       </c>
       <c r="Z7">
@@ -1168,8 +1178,11 @@
       <c r="AA7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AB7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1179,26 +1192,26 @@
       <c r="G8">
         <v>2</v>
       </c>
-      <c r="L8">
-        <v>2</v>
-      </c>
       <c r="M8">
         <v>2</v>
       </c>
-      <c r="O8">
-        <v>2</v>
-      </c>
-      <c r="S8">
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="P8">
+        <v>2</v>
+      </c>
+      <c r="T8">
         <v>8</v>
       </c>
-      <c r="T8">
-        <v>2</v>
-      </c>
       <c r="U8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="V8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1208,23 +1221,23 @@
       <c r="G9">
         <v>4</v>
       </c>
-      <c r="L9">
-        <v>3</v>
-      </c>
       <c r="M9">
         <v>3</v>
       </c>
-      <c r="O9">
-        <v>3</v>
-      </c>
-      <c r="S9">
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="P9">
+        <v>3</v>
+      </c>
+      <c r="T9">
         <v>9</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1252,20 +1265,20 @@
       <c r="K10">
         <v>5</v>
       </c>
-      <c r="S10">
-        <v>6</v>
-      </c>
-      <c r="V10">
-        <v>5</v>
+      <c r="T10">
+        <v>6</v>
       </c>
       <c r="W10">
         <v>5</v>
       </c>
-      <c r="Z10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="X10">
+        <v>5</v>
+      </c>
+      <c r="AA10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1293,26 +1306,26 @@
       <c r="K11">
         <v>2</v>
       </c>
-      <c r="S11">
-        <v>2</v>
-      </c>
-      <c r="V11">
+      <c r="T11">
         <v>2</v>
       </c>
       <c r="W11">
         <v>2</v>
       </c>
-      <c r="Y11">
-        <v>4</v>
+      <c r="X11">
+        <v>2</v>
       </c>
       <c r="Z11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AA11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="AB11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1340,23 +1353,23 @@
       <c r="K12">
         <v>6</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>7</v>
       </c>
-      <c r="U12">
-        <v>6</v>
-      </c>
       <c r="V12">
         <v>6</v>
       </c>
       <c r="W12">
         <v>6</v>
       </c>
-      <c r="Z12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="X12">
+        <v>6</v>
+      </c>
+      <c r="AA12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1384,29 +1397,29 @@
       <c r="K13">
         <v>4</v>
       </c>
-      <c r="S13">
-        <v>4</v>
-      </c>
-      <c r="U13">
+      <c r="T13">
         <v>4</v>
       </c>
       <c r="V13">
         <v>4</v>
       </c>
       <c r="W13">
-        <v>3</v>
-      </c>
-      <c r="Y13">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="X13">
+        <v>3</v>
       </c>
       <c r="Z13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AA13">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AB13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1431,20 +1444,17 @@
       <c r="K14">
         <v>1</v>
       </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
       <c r="M14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O14">
-        <v>4</v>
-      </c>
-      <c r="S14">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>4</v>
       </c>
       <c r="T14">
         <v>1</v>
@@ -1453,10 +1463,10 @@
         <v>1</v>
       </c>
       <c r="V14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X14">
         <v>1</v>
@@ -1474,43 +1484,46 @@
         <v>1</v>
       </c>
       <c r="AC14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AD14">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AE14">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AF14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AG14">
         <v>1</v>
       </c>
-      <c r="AI14">
-        <v>2</v>
+      <c r="AH14">
+        <v>1</v>
       </c>
       <c r="AJ14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AL14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AM14">
         <v>1</v>
       </c>
       <c r="AN14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AO14">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AP14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1538,13 +1551,10 @@
       <c r="K15">
         <v>5</v>
       </c>
-      <c r="L15">
-        <v>5</v>
-      </c>
       <c r="M15">
-        <v>6</v>
-      </c>
-      <c r="O15">
+        <v>5</v>
+      </c>
+      <c r="N15">
         <v>6</v>
       </c>
       <c r="P15">
@@ -1557,43 +1567,43 @@
         <v>6</v>
       </c>
       <c r="S15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="T15">
         <v>7</v>
       </c>
       <c r="U15">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="V15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W15">
-        <v>5</v>
-      </c>
-      <c r="Z15">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="X15">
+        <v>5</v>
       </c>
       <c r="AA15">
         <v>4</v>
       </c>
       <c r="AB15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AC15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AD15">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AE15">
-        <v>6</v>
-      </c>
-      <c r="AI15">
-        <v>4</v>
-      </c>
-      <c r="AK15">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="AF15">
+        <v>6</v>
+      </c>
+      <c r="AJ15">
+        <v>4</v>
       </c>
       <c r="AL15">
         <v>3</v>
@@ -1607,8 +1617,11 @@
       <c r="AO15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="AP15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1624,10 +1637,10 @@
       <c r="I16">
         <v>1</v>
       </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
-      <c r="O16">
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="N16">
         <v>1</v>
       </c>
       <c r="P16">
@@ -1640,22 +1653,22 @@
         <v>1</v>
       </c>
       <c r="S16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V16">
-        <v>4</v>
-      </c>
-      <c r="AB16">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="W16">
+        <v>4</v>
       </c>
       <c r="AC16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD16">
         <v>1</v>
@@ -1663,26 +1676,29 @@
       <c r="AE16">
         <v>1</v>
       </c>
-      <c r="AH16">
+      <c r="AF16">
         <v>1</v>
       </c>
       <c r="AI16">
         <v>1</v>
       </c>
-      <c r="AK16">
-        <v>1</v>
-      </c>
-      <c r="AN16">
-        <v>2</v>
+      <c r="AJ16">
+        <v>1</v>
+      </c>
+      <c r="AL16">
+        <v>1</v>
       </c>
       <c r="AO16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AP16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AQ16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1713,13 +1729,10 @@
       <c r="K17">
         <v>2</v>
       </c>
-      <c r="L17">
-        <v>2</v>
-      </c>
       <c r="M17">
         <v>2</v>
       </c>
-      <c r="O17">
+      <c r="N17">
         <v>2</v>
       </c>
       <c r="P17">
@@ -1741,13 +1754,13 @@
         <v>2</v>
       </c>
       <c r="V17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W17">
-        <v>3</v>
-      </c>
-      <c r="Y17">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="X17">
+        <v>3</v>
       </c>
       <c r="Z17">
         <v>2</v>
@@ -1756,25 +1769,25 @@
         <v>2</v>
       </c>
       <c r="AB17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AC17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD17">
         <v>2</v>
       </c>
       <c r="AE17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AF17">
-        <v>2</v>
-      </c>
-      <c r="AI17">
-        <v>3</v>
-      </c>
-      <c r="AK17">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="AG17">
+        <v>2</v>
+      </c>
+      <c r="AJ17">
+        <v>3</v>
       </c>
       <c r="AL17">
         <v>2</v>
@@ -1783,13 +1796,16 @@
         <v>2</v>
       </c>
       <c r="AN17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AO17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="AP17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1817,38 +1833,38 @@
       <c r="K18">
         <v>4</v>
       </c>
-      <c r="L18">
-        <v>3</v>
-      </c>
       <c r="M18">
-        <v>4</v>
-      </c>
-      <c r="O18">
-        <v>3</v>
-      </c>
-      <c r="S18">
+        <v>3</v>
+      </c>
+      <c r="N18">
+        <v>4</v>
+      </c>
+      <c r="P18">
+        <v>3</v>
+      </c>
+      <c r="T18">
         <v>8</v>
       </c>
-      <c r="T18">
-        <v>3</v>
-      </c>
-      <c r="V18">
+      <c r="U18">
+        <v>3</v>
+      </c>
+      <c r="W18">
         <v>7</v>
       </c>
-      <c r="W18">
-        <v>6</v>
-      </c>
-      <c r="AD18">
+      <c r="X18">
+        <v>6</v>
+      </c>
+      <c r="AE18">
         <v>9</v>
       </c>
-      <c r="AJ18">
-        <v>3</v>
-      </c>
       <c r="AK18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="AL18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1876,17 +1892,14 @@
       <c r="K19">
         <v>3</v>
       </c>
-      <c r="L19">
-        <v>4</v>
-      </c>
       <c r="M19">
-        <v>5</v>
-      </c>
-      <c r="O19">
+        <v>4</v>
+      </c>
+      <c r="N19">
         <v>5</v>
       </c>
       <c r="P19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q19">
         <v>4</v>
@@ -1895,16 +1908,16 @@
         <v>4</v>
       </c>
       <c r="S19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T19">
         <v>5</v>
       </c>
       <c r="U19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="V19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W19">
         <v>2</v>
@@ -1913,40 +1926,40 @@
         <v>2</v>
       </c>
       <c r="Y19">
-        <v>4</v>
-      </c>
-      <c r="AA19">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="Z19">
+        <v>4</v>
       </c>
       <c r="AB19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AC19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE19">
-        <v>2</v>
-      </c>
-      <c r="AI19">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="AF19">
+        <v>2</v>
       </c>
       <c r="AJ19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="AK19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
       <c r="B20" t="s">
         <v>43</v>
       </c>
-      <c r="P20">
-        <v>5</v>
-      </c>
       <c r="Q20">
         <v>5</v>
       </c>
@@ -1954,7 +1967,7 @@
         <v>5</v>
       </c>
       <c r="S20">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T20">
         <v>6</v>
@@ -1963,66 +1976,66 @@
         <v>6</v>
       </c>
       <c r="V20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W20">
+        <v>5</v>
+      </c>
+      <c r="X20">
         <v>7</v>
       </c>
-      <c r="Y20">
-        <v>5</v>
-      </c>
       <c r="Z20">
         <v>5</v>
       </c>
-      <c r="AC20">
+      <c r="AA20">
         <v>5</v>
       </c>
       <c r="AD20">
         <v>5</v>
       </c>
       <c r="AE20">
+        <v>5</v>
+      </c>
+      <c r="AF20">
         <v>7</v>
       </c>
-      <c r="AI20">
-        <v>6</v>
-      </c>
       <c r="AJ20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="AK20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
       <c r="B21" t="s">
         <v>43</v>
       </c>
-      <c r="P21">
-        <v>7</v>
-      </c>
       <c r="Q21">
         <v>7</v>
       </c>
       <c r="R21">
         <v>7</v>
       </c>
-      <c r="AD21">
+      <c r="S21">
+        <v>7</v>
+      </c>
+      <c r="AE21">
         <v>8</v>
       </c>
-      <c r="AJ21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AK21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
       <c r="B22" t="s">
         <v>43</v>
       </c>
-      <c r="P22">
-        <v>3</v>
-      </c>
       <c r="Q22">
         <v>3</v>
       </c>
@@ -2030,16 +2043,16 @@
         <v>3</v>
       </c>
       <c r="S22">
-        <v>4</v>
-      </c>
-      <c r="U22">
+        <v>3</v>
+      </c>
+      <c r="T22">
+        <v>4</v>
+      </c>
+      <c r="V22">
         <v>7</v>
       </c>
-      <c r="W22">
-        <v>4</v>
-      </c>
-      <c r="Y22">
-        <v>3</v>
+      <c r="X22">
+        <v>4</v>
       </c>
       <c r="Z22">
         <v>3</v>
@@ -2047,16 +2060,19 @@
       <c r="AA22">
         <v>3</v>
       </c>
-      <c r="AD22">
+      <c r="AB22">
+        <v>3</v>
+      </c>
+      <c r="AE22">
         <v>7</v>
       </c>
-      <c r="AE22">
+      <c r="AF22">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:AG1"/>
+    <mergeCell ref="C1:AH1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -2065,24 +2081,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="74.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -2090,42 +2106,42 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -2136,7 +2152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>42327</v>
       </c>
@@ -2147,7 +2163,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>42344</v>
       </c>
@@ -2158,7 +2174,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>42403</v>
       </c>
@@ -2169,7 +2185,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>42607</v>
       </c>
@@ -2180,7 +2196,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>42624</v>
       </c>
@@ -2191,7 +2207,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>42709</v>
       </c>
@@ -2202,7 +2218,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>42719</v>
       </c>
@@ -2213,7 +2229,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>42758</v>
       </c>
@@ -2224,7 +2240,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>42769</v>
       </c>
@@ -2235,7 +2251,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>42779</v>
       </c>
@@ -2246,7 +2262,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>42964</v>
       </c>
@@ -2257,7 +2273,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>42965</v>
       </c>
@@ -2266,6 +2282,14 @@
       </c>
       <c r="C25" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>43013</v>
+      </c>
+      <c r="B26" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>